<commit_message>
Updated German template listem from 2 to 3. Also, updated test cases sheet with new rows and columns for Battery Standby for FC test cases
</commit_message>
<xml_diff>
--- a/Test Data/TC_52210_11_12_13_Verify_Power_Calculation_Is_Populated_Where_Error_And_Warning_Messages_Are_Displayed.xlsx
+++ b/Test Data/TC_52210_11_12_13_Verify_Power_Calculation_Is_Populated_Where_Error_And_Warning_Messages_Are_Displayed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA1FD8E-51FB-43A5-83C3-AD4BF5A9D130}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CD26CD-8D2C-4C5B-B687-975BD1E97091}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24V_And_SystemLoad" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="52">
   <si>
     <t>Label</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Load at 24V has reached 95% for panel Node1-Pro32xD,System load has reached 100% for panel Node1-Pro32xD</t>
+  </si>
+  <si>
+    <t>Loading Details Name</t>
+  </si>
+  <si>
+    <t>Main Processor 24V (A)</t>
   </si>
 </sst>
 </file>
@@ -638,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,6 +655,7 @@
     <col min="3" max="3" width="31.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.109375" customWidth="1"/>
     <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -659,7 +666,9 @@
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
       <c r="E1" s="19"/>
-      <c r="G1" s="9"/>
+      <c r="G1" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="H1" s="9"/>
       <c r="I1" s="10"/>
     </row>
@@ -675,6 +684,9 @@
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="11"/>
+      <c r="G2" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -1075,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D039028F-250C-43A1-A01D-74387B073A3C}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>